<commit_message>
Add NPA text as description body.
</commit_message>
<xml_diff>
--- a/dashboard_loader/skills_reform_uploader/skills_reform.xlsx
+++ b/dashboard_loader/skills_reform_uploader/skills_reform.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="46">
   <si>
     <t xml:space="preserve">National Partnership Agreement on Skills Reform</t>
   </si>
@@ -153,6 +153,12 @@
   </si>
   <si>
     <t xml:space="preserve">Updated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desc Body</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Commonwealth committed $1.75 billion over five years for a National Partnership Agreement on Skills Reform (NPASR) to reform the vocational education and training system. The NPASR commenced in 2012 and expires in June 2017.</t>
   </si>
 </sst>
 </file>
@@ -162,7 +168,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -216,6 +222,13 @@
       <family val="1"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val=""/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -280,7 +293,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -322,6 +335,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -404,8 +421,8 @@
   </sheetPr>
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -961,10 +978,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1006,6 +1023,14 @@
         <v>2016</v>
       </c>
     </row>
+    <row r="5" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>